<commit_message>
refactor: Improve Export to Excel functionality in Report page
</commit_message>
<xml_diff>
--- a/DC/Template/5SReportTemplate.xlsx
+++ b/DC/Template/5SReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DC\DC\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A165728-A984-4A00-9DCF-3C0CB144207F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCA209E-1AE1-4002-87E8-B7C44019506F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
   </bookViews>
@@ -144,17 +144,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,59 +498,62 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="13.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="4"/>
-    <col min="6" max="6" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="11.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="19" style="9" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: Add ranking to the report
</commit_message>
<xml_diff>
--- a/DC/Template/5SReportTemplate.xlsx
+++ b/DC/Template/5SReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DC\DC\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCA209E-1AE1-4002-87E8-B7C44019506F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F7A1C-04DF-46CB-A30E-8556713775D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Score Report" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -50,22 +50,25 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Average Score:</t>
-  </si>
-  <si>
-    <t>Number of Graded staff:</t>
-  </si>
-  <si>
     <t>Survey:</t>
   </si>
   <si>
-    <t>Export time:</t>
-  </si>
-  <si>
-    <t>Highest Score:</t>
-  </si>
-  <si>
-    <t>Lowest Score:</t>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Average score:</t>
+  </si>
+  <si>
+    <t>Number of graded staff:</t>
+  </si>
+  <si>
+    <t>Highest score:</t>
+  </si>
+  <si>
+    <t>Lowest score:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export time: </t>
   </si>
 </sst>
 </file>
@@ -144,23 +147,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,72 +494,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1BFAB6-9A29-441B-8832-A3DFFBFCE6DD}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19" style="9" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="11.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F4" s="3" t="s">
-        <v>5</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: update template layout
</commit_message>
<xml_diff>
--- a/DC/Template/5SReportTemplate.xlsx
+++ b/DC/Template/5SReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DC\DC\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F7A1C-04DF-46CB-A30E-8556713775D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60C0496-4B46-4B22-95B3-4D088367AEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Score Report" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Survey:</t>
-  </si>
-  <si>
     <t>Ranking</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">Export time: </t>
+  </si>
+  <si>
+    <t>Survey</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -159,6 +159,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,7 +500,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -515,22 +518,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
       <c r="G1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -545,18 +548,18 @@
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Update GradingDialog and ReportShowDetailDialog components
</commit_message>
<xml_diff>
--- a/DC/Template/5SReportTemplate.xlsx
+++ b/DC/Template/5SReportTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DC\DC\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D0B5FC-B0C6-41BA-ADBF-C51388FC405E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC836D13-B9AC-4A58-8BCE-834C6B51F16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
   </bookViews>
@@ -530,19 +530,18 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="19" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="26.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -589,6 +588,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E3" s="7"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E4" s="7"/>
@@ -598,6 +598,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E5" s="7"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E6" s="7"/>

</xml_diff>

<commit_message>
refactor: Update App.razor, Dialog/ReportShowDetailDialog.razor.cs, Pages/Account/Login.razor.cs, and Pages/Question.razor to improve code readability and maintainability
</commit_message>
<xml_diff>
--- a/DC/Template/5SReportTemplate.xlsx
+++ b/DC/Template/5SReportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DC\DC\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC836D13-B9AC-4A58-8BCE-834C6B51F16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE03F7-B135-4B1D-AB97-734D36653C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6A343F2-45D9-4B5A-A157-1934E6D4337E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -186,6 +189,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1BFAB6-9A29-441B-8832-A3DFFBFCE6DD}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -538,7 +544,7 @@
     <col min="1" max="2" width="11.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="19" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="7" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="35.7109375" style="3" customWidth="1"/>
@@ -547,18 +553,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="G1" s="10" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="G1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -573,7 +579,7 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -587,27 +593,24 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>